<commit_message>
extracted all the file
</commit_message>
<xml_diff>
--- a/MFIC/MFIC__sec_filing_links.xlsx
+++ b/MFIC/MFIC__sec_filing_links.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fuadhassan/Desktop/BDC_RA/MFIC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C2529A1-2870-2D42-9C18-AAB0D62E1BF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6709A553-DC90-CE48-9A61-2EEB7DD6146B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -352,9 +352,6 @@
     <t>2015-03-31</t>
   </si>
   <si>
-    <t>https://www.sec.gov/Archives/edgar/data/0001278752/000127875215000011/ainv-2015331x10ka.htm</t>
-  </si>
-  <si>
     <t>2015-02-05</t>
   </si>
   <si>
@@ -440,6 +437,9 @@
   </si>
   <si>
     <t>https://www.sec.gov/Archives/edgar/data/1278752/000095017022021830/mfic-20220930.htm</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/1278752/000127875215000008/ainv-2015331x10k.htm</t>
   </si>
 </sst>
 </file>
@@ -816,8 +816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="144" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -860,7 +860,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -877,7 +877,7 @@
         <v>10</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -894,7 +894,7 @@
         <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -911,7 +911,7 @@
         <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -928,7 +928,7 @@
         <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1438,7 +1438,7 @@
         <v>109</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>110</v>
+        <v>139</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -1449,13 +1449,13 @@
         <v>6</v>
       </c>
       <c r="C37" t="s">
+        <v>110</v>
+      </c>
+      <c r="D37" t="s">
         <v>111</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="E37" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -1466,13 +1466,13 @@
         <v>6</v>
       </c>
       <c r="C38" t="s">
+        <v>113</v>
+      </c>
+      <c r="D38" t="s">
         <v>114</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>115</v>
-      </c>
-      <c r="E38" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -1483,13 +1483,13 @@
         <v>6</v>
       </c>
       <c r="C39" t="s">
+        <v>116</v>
+      </c>
+      <c r="D39" t="s">
         <v>117</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>118</v>
-      </c>
-      <c r="E39" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -1500,13 +1500,13 @@
         <v>23</v>
       </c>
       <c r="C40" t="s">
+        <v>119</v>
+      </c>
+      <c r="D40" t="s">
         <v>120</v>
       </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
         <v>121</v>
-      </c>
-      <c r="E40" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -1517,13 +1517,13 @@
         <v>6</v>
       </c>
       <c r="C41" t="s">
+        <v>122</v>
+      </c>
+      <c r="D41" t="s">
         <v>123</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
         <v>124</v>
-      </c>
-      <c r="E41" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -1534,13 +1534,13 @@
         <v>6</v>
       </c>
       <c r="C42" t="s">
+        <v>125</v>
+      </c>
+      <c r="D42" t="s">
         <v>126</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
         <v>127</v>
-      </c>
-      <c r="E42" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -1551,13 +1551,13 @@
         <v>23</v>
       </c>
       <c r="C43" t="s">
+        <v>128</v>
+      </c>
+      <c r="D43" t="s">
         <v>129</v>
       </c>
-      <c r="D43" t="s">
+      <c r="E43" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -1568,13 +1568,13 @@
         <v>6</v>
       </c>
       <c r="C44" t="s">
+        <v>131</v>
+      </c>
+      <c r="D44" t="s">
         <v>132</v>
       </c>
-      <c r="D44" t="s">
+      <c r="E44" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -1583,7 +1583,7 @@
     <hyperlink ref="E3" r:id="rId2" xr:uid="{E1C111B7-46CC-0E4A-9828-D5FDF1BEB476}"/>
     <hyperlink ref="E44" r:id="rId3" xr:uid="{80E54DBD-71C3-8045-8E03-C240D2C61904}"/>
     <hyperlink ref="E43" r:id="rId4" xr:uid="{03D42C88-DBBC-1145-960D-986F80CA0D99}"/>
-    <hyperlink ref="E36" r:id="rId5" xr:uid="{932D80E9-78C9-B94A-B97F-B063830654DA}"/>
+    <hyperlink ref="E37" r:id="rId5" xr:uid="{A3E691AE-677A-C042-81BE-614B3A0D57FB}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>